<commit_message>
Cambié la escala de los pesos de 2.1.7 y los puse del 1 al 3. Las curvas se tocan tal vez demasiado, y en algunos puntos tienen pendientes muy pronunciadas, me gustaría que lo miren y den su opinión.
</commit_message>
<xml_diff>
--- a/ejercicios/Indicadores/2.1.7.xlsx
+++ b/ejercicios/Indicadores/2.1.7.xlsx
@@ -78,13 +78,13 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>Acum desa estim</t>
-  </si>
-  <si>
-    <t>Acum QC estim</t>
-  </si>
-  <si>
-    <t>Acum acep estim</t>
+    <t>FC desa. estimado</t>
+  </si>
+  <si>
+    <t>FC QC estimado</t>
+  </si>
+  <si>
+    <t>FC usuario estimado</t>
   </si>
 </sst>
 </file>
@@ -353,93 +353,99 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Acum desa estim</c:v>
+                  <c:v>FC desa. estimado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>FC!$M$4:$M$29</c:f>
+              <c:f>FC!$M$4:$M$30</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>38718</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>38790</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>38797</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>38804</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>38806</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>38808</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>38817</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>38838</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38852</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>38901</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>38910</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>38930</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>39026</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>39071</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>39097</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>39216</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>39223</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>39265</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>39279</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>39284</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>39293</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>39295</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>39301</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>39326</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>39386</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>39428</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>39446</c:v>
                 </c:pt>
               </c:numCache>
@@ -447,87 +453,90 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FC!$N$4:$N$29</c:f>
+              <c:f>FC!$N$4:$N$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>64</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>76</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>106</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>106</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>106</c:v>
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -542,93 +551,99 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Acum QC estim</c:v>
+                  <c:v>FC QC estimado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>FC!$M$4:$M$29</c:f>
+              <c:f>FC!$M$4:$M$30</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>38718</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>38790</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>38797</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>38804</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>38806</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>38808</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>38817</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>38838</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38852</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>38901</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>38910</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>38930</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>39026</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>39071</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>39097</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>39216</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>39223</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>39265</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>39279</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>39284</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>39293</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>39295</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>39301</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>39326</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>39386</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>39428</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>39446</c:v>
                 </c:pt>
               </c:numCache>
@@ -636,10 +651,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FC!$O$4:$O$29</c:f>
+              <c:f>FC!$O$4:$O$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -647,76 +662,79 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>64</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>68</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>76</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>106</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>106</c:v>
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -731,93 +749,99 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Acum acep estim</c:v>
+                  <c:v>FC usuario estimado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>FC!$M$4:$M$29</c:f>
+              <c:f>FC!$M$4:$M$30</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>38718</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>38790</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>38797</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>38804</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>38806</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>38808</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>38817</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>38838</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38852</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>38901</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>38910</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>38930</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>39026</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>39071</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>39097</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>39216</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>39223</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>39265</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>39279</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>39284</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>39293</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>39295</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>39301</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>39326</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>39386</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>39428</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>39446</c:v>
                 </c:pt>
               </c:numCache>
@@ -825,10 +849,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FC!$P$4:$P$29</c:f>
+              <c:f>FC!$P$4:$P$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -848,88 +872,91 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>38</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>46</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>76</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>76</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>106</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="48845184"/>
-        <c:axId val="48848256"/>
+        <c:axId val="59599872"/>
+        <c:axId val="59626240"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="48845184"/>
+        <c:axId val="59599872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48848256"/>
+        <c:crossAx val="59626240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="48848256"/>
+        <c:axId val="59626240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +964,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48845184"/>
+        <c:crossAx val="59599872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -950,7 +977,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -960,14 +987,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>761999</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -1279,7 +1306,7 @@
   <dimension ref="B1:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1299,7 +1326,7 @@
       </c>
     </row>
     <row r="2" spans="2:19" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:19" s="1" customFormat="1" ht="30.75" thickBot="1">
+    <row r="3" spans="2:19" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1">
       <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1340,21 +1367,18 @@
         <v>22</v>
       </c>
       <c r="R3"/>
-      <c r="S3" t="str">
-        <f>D3</f>
-        <v>Acumulado</v>
-      </c>
+      <c r="S3"/>
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="9">
         <f>SUM($C$4:C4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="11">
         <v>38790</v>
@@ -1369,11 +1393,10 @@
       </c>
       <c r="J4" s="10"/>
       <c r="M4" s="17">
-        <f>E4</f>
-        <v>38790</v>
+        <v>38718</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1381,14 +1404,7 @@
       <c r="P4">
         <v>0</v>
       </c>
-      <c r="R4" s="17">
-        <f>E4</f>
-        <v>38790</v>
-      </c>
-      <c r="S4">
-        <f>D4</f>
-        <v>3</v>
-      </c>
+      <c r="R4" s="17"/>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="3" t="s">
@@ -1399,7 +1415,7 @@
       </c>
       <c r="D5" s="2">
         <f>SUM($C$4:C5)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="12">
         <v>38797</v>
@@ -1414,11 +1430,11 @@
       </c>
       <c r="J5" s="4"/>
       <c r="M5" s="17">
-        <f>E5</f>
-        <v>38797</v>
+        <f>E4</f>
+        <v>38790</v>
       </c>
       <c r="N5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1426,25 +1442,18 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="R5" s="17">
-        <f>E5</f>
-        <v>38797</v>
-      </c>
-      <c r="S5">
-        <f>D5</f>
-        <v>4</v>
-      </c>
+      <c r="R5" s="17"/>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2">
         <f>SUM($C$4:C6)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E6" s="12">
         <v>38808</v>
@@ -1459,37 +1468,30 @@
       </c>
       <c r="J6" s="4"/>
       <c r="M6" s="17">
-        <f>G5</f>
-        <v>38804</v>
+        <f>E5</f>
+        <v>38797</v>
       </c>
       <c r="N6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="R6" s="17">
-        <f>E6</f>
-        <v>38808</v>
-      </c>
-      <c r="S6">
-        <f>D6</f>
-        <v>6</v>
-      </c>
+      <c r="R6" s="17"/>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
         <f>SUM($C$4:C7)</f>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E7" s="12">
         <v>38901</v>
@@ -1504,37 +1506,30 @@
       </c>
       <c r="J7" s="4"/>
       <c r="M7" s="17">
-        <f>G4</f>
-        <v>38806</v>
+        <f>G5</f>
+        <v>38804</v>
       </c>
       <c r="N7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
-      <c r="R7" s="17">
-        <f>E7</f>
-        <v>38901</v>
-      </c>
-      <c r="S7">
-        <f>D7</f>
-        <v>18</v>
-      </c>
+      <c r="R7" s="17"/>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2">
         <f>SUM($C$4:C8)</f>
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E8" s="12">
         <v>39026</v>
@@ -1549,37 +1544,30 @@
       </c>
       <c r="J8" s="4"/>
       <c r="M8" s="17">
-        <f>E6</f>
-        <v>38808</v>
+        <f>G4</f>
+        <v>38806</v>
       </c>
       <c r="N8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
-      <c r="R8" s="17">
-        <f>E8</f>
-        <v>39026</v>
-      </c>
-      <c r="S8">
-        <f>D8</f>
-        <v>34</v>
-      </c>
+      <c r="R8" s="17"/>
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2">
         <f>SUM($C$4:C9)</f>
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="E9" s="12">
         <v>39216</v>
@@ -1594,37 +1582,30 @@
       </c>
       <c r="J9" s="4"/>
       <c r="M9" s="17">
-        <f>G6</f>
-        <v>38817</v>
+        <f>E6</f>
+        <v>38808</v>
       </c>
       <c r="N9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
-      <c r="R9" s="17">
-        <f>E9</f>
-        <v>39216</v>
-      </c>
-      <c r="S9">
-        <f>D9</f>
-        <v>64</v>
-      </c>
+      <c r="R9" s="17"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
         <f>SUM($C$4:C10)</f>
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E10" s="12">
         <v>39223</v>
@@ -1639,37 +1620,30 @@
       </c>
       <c r="J10" s="4"/>
       <c r="M10" s="17">
-        <f>I4</f>
-        <v>38838</v>
+        <f>G6</f>
+        <v>38817</v>
       </c>
       <c r="N10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P10">
-        <v>4</v>
-      </c>
-      <c r="R10" s="17">
-        <f>E10</f>
-        <v>39223</v>
-      </c>
-      <c r="S10">
-        <f>D10</f>
-        <v>68</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R10" s="17"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2">
         <f>SUM($C$4:C11)</f>
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="E11" s="12">
         <v>39265</v>
@@ -1684,37 +1658,30 @@
       </c>
       <c r="J11" s="4"/>
       <c r="M11" s="17">
-        <f>I6</f>
-        <v>38852</v>
+        <f>I4</f>
+        <v>38838</v>
       </c>
       <c r="N11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P11">
-        <v>6</v>
-      </c>
-      <c r="R11" s="17">
-        <f>E11</f>
-        <v>39265</v>
-      </c>
-      <c r="S11">
-        <f>D11</f>
-        <v>76</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="R11" s="17"/>
     </row>
     <row r="12" spans="2:19" ht="15.75" thickBot="1">
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="6">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D12" s="6">
         <f>SUM($C$4:C12)</f>
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="E12" s="16">
         <v>39386</v>
@@ -1729,284 +1696,289 @@
       </c>
       <c r="J12" s="7"/>
       <c r="M12" s="17">
+        <f>I6</f>
+        <v>38852</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="R12" s="17"/>
+    </row>
+    <row r="13" spans="2:19">
+      <c r="M13" s="17">
         <f>E7</f>
         <v>38901</v>
       </c>
-      <c r="N12">
-        <v>18</v>
-      </c>
-      <c r="O12">
-        <v>6</v>
-      </c>
-      <c r="P12">
-        <v>6</v>
-      </c>
-      <c r="R12" s="17">
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19">
+      <c r="M14" s="17">
+        <f>G7</f>
+        <v>38910</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19">
+      <c r="M15" s="17">
+        <f>I7</f>
+        <v>38930</v>
+      </c>
+      <c r="N15">
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19">
+      <c r="M16" s="17">
+        <f>E8</f>
+        <v>39026</v>
+      </c>
+      <c r="N16">
+        <v>7</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="13:16">
+      <c r="M17" s="17">
+        <f>G8</f>
+        <v>39071</v>
+      </c>
+      <c r="N17">
+        <v>7</v>
+      </c>
+      <c r="O17">
+        <v>7</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="13:16">
+      <c r="M18" s="17">
+        <f>I8</f>
+        <v>39097</v>
+      </c>
+      <c r="N18">
+        <v>7</v>
+      </c>
+      <c r="O18">
+        <v>7</v>
+      </c>
+      <c r="P18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="13:16">
+      <c r="M19" s="17">
+        <f>E9</f>
+        <v>39216</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>7</v>
+      </c>
+      <c r="P19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="13:16">
+      <c r="M20" s="17">
+        <f>E10</f>
+        <v>39223</v>
+      </c>
+      <c r="N20">
+        <v>11</v>
+      </c>
+      <c r="O20">
+        <v>7</v>
+      </c>
+      <c r="P20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="13:16">
+      <c r="M21" s="17">
+        <f>E11</f>
+        <v>39265</v>
+      </c>
+      <c r="N21">
+        <v>12</v>
+      </c>
+      <c r="O21">
+        <v>7</v>
+      </c>
+      <c r="P21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="13:16">
+      <c r="M22" s="17">
+        <f>G9</f>
+        <v>39279</v>
+      </c>
+      <c r="N22">
+        <v>12</v>
+      </c>
+      <c r="O22">
+        <v>10</v>
+      </c>
+      <c r="P22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="13:16">
+      <c r="M23" s="17">
+        <f>G10</f>
+        <v>39284</v>
+      </c>
+      <c r="N23">
+        <v>12</v>
+      </c>
+      <c r="O23">
+        <v>11</v>
+      </c>
+      <c r="P23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="13:16">
+      <c r="M24" s="17">
+        <f>G11</f>
+        <v>39293</v>
+      </c>
+      <c r="N24">
+        <v>12</v>
+      </c>
+      <c r="O24">
+        <v>12</v>
+      </c>
+      <c r="P24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="13:16">
+      <c r="M25" s="17">
+        <f>I10</f>
+        <v>39295</v>
+      </c>
+      <c r="N25">
+        <v>12</v>
+      </c>
+      <c r="O25">
+        <v>12</v>
+      </c>
+      <c r="P25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="13:16">
+      <c r="M26" s="17">
+        <f>I11</f>
+        <v>39301</v>
+      </c>
+      <c r="N26">
+        <v>12</v>
+      </c>
+      <c r="O26">
+        <v>12</v>
+      </c>
+      <c r="P26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="13:16">
+      <c r="M27" s="17">
+        <f>I9</f>
+        <v>39326</v>
+      </c>
+      <c r="N27">
+        <v>12</v>
+      </c>
+      <c r="O27">
+        <v>12</v>
+      </c>
+      <c r="P27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="13:16">
+      <c r="M28" s="17">
         <f>E12</f>
         <v>39386</v>
       </c>
-      <c r="S12">
-        <f>D12</f>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19">
-      <c r="M13" s="17">
-        <f>G7</f>
-        <v>38910</v>
-      </c>
-      <c r="N13">
-        <v>18</v>
-      </c>
-      <c r="O13">
-        <v>18</v>
-      </c>
-      <c r="P13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19">
-      <c r="M14" s="17">
-        <f>I7</f>
-        <v>38930</v>
-      </c>
-      <c r="N14">
-        <v>18</v>
-      </c>
-      <c r="O14">
-        <v>18</v>
-      </c>
-      <c r="P14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19">
-      <c r="M15" s="17">
-        <f>E8</f>
-        <v>39026</v>
-      </c>
-      <c r="N15">
-        <v>34</v>
-      </c>
-      <c r="O15">
-        <v>18</v>
-      </c>
-      <c r="P15">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19">
-      <c r="M16" s="17">
-        <f>G8</f>
-        <v>39071</v>
-      </c>
-      <c r="N16">
-        <v>34</v>
-      </c>
-      <c r="O16">
-        <v>34</v>
-      </c>
-      <c r="P16">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="13:16">
-      <c r="M17" s="17">
-        <f>I8</f>
-        <v>39097</v>
-      </c>
-      <c r="N17">
-        <v>34</v>
-      </c>
-      <c r="O17">
-        <v>34</v>
-      </c>
-      <c r="P17">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="13:16">
-      <c r="M18" s="17">
-        <f>E9</f>
-        <v>39216</v>
-      </c>
-      <c r="N18">
-        <v>64</v>
-      </c>
-      <c r="O18">
-        <v>34</v>
-      </c>
-      <c r="P18">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="13:16">
-      <c r="M19" s="17">
-        <f>E10</f>
-        <v>39223</v>
-      </c>
-      <c r="N19">
-        <v>68</v>
-      </c>
-      <c r="O19">
-        <v>34</v>
-      </c>
-      <c r="P19">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="13:16">
-      <c r="M20" s="17">
-        <f>E11</f>
-        <v>39265</v>
-      </c>
-      <c r="N20">
-        <v>76</v>
-      </c>
-      <c r="O20">
-        <v>34</v>
-      </c>
-      <c r="P20">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="13:16">
-      <c r="M21" s="17">
-        <f>G9</f>
-        <v>39279</v>
-      </c>
-      <c r="N21">
-        <v>76</v>
-      </c>
-      <c r="O21">
-        <v>64</v>
-      </c>
-      <c r="P21">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="13:16">
-      <c r="M22" s="17">
-        <f>G10</f>
-        <v>39284</v>
-      </c>
-      <c r="N22">
-        <v>76</v>
-      </c>
-      <c r="O22">
-        <v>68</v>
-      </c>
-      <c r="P22">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="13:16">
-      <c r="M23" s="17">
-        <f>G11</f>
-        <v>39293</v>
-      </c>
-      <c r="N23">
-        <v>76</v>
-      </c>
-      <c r="O23">
-        <v>76</v>
-      </c>
-      <c r="P23">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="13:16">
-      <c r="M24" s="17">
-        <f>I10</f>
-        <v>39295</v>
-      </c>
-      <c r="N24">
-        <v>76</v>
-      </c>
-      <c r="O24">
-        <v>76</v>
-      </c>
-      <c r="P24">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="13:16">
-      <c r="M25" s="17">
-        <f>I11</f>
-        <v>39301</v>
-      </c>
-      <c r="N25">
-        <v>76</v>
-      </c>
-      <c r="O25">
-        <v>76</v>
-      </c>
-      <c r="P25">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="13:16">
-      <c r="M26" s="17">
-        <f>I9</f>
-        <v>39326</v>
-      </c>
-      <c r="N26">
-        <v>76</v>
-      </c>
-      <c r="O26">
-        <v>76</v>
-      </c>
-      <c r="P26">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="13:16">
-      <c r="M27" s="17">
-        <f>E12</f>
-        <v>39386</v>
-      </c>
-      <c r="N27">
-        <v>106</v>
-      </c>
-      <c r="O27">
-        <v>76</v>
-      </c>
-      <c r="P27">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="13:16">
-      <c r="M28" s="17">
+      <c r="N28">
+        <v>15</v>
+      </c>
+      <c r="O28">
+        <v>12</v>
+      </c>
+      <c r="P28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="13:16">
+      <c r="M29" s="17">
         <f>G12</f>
         <v>39428</v>
       </c>
-      <c r="N28">
-        <v>106</v>
-      </c>
-      <c r="O28">
-        <v>106</v>
-      </c>
-      <c r="P28">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="13:16">
-      <c r="M29" s="17">
+      <c r="N29">
+        <v>15</v>
+      </c>
+      <c r="O29">
+        <v>15</v>
+      </c>
+      <c r="P29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="13:16">
+      <c r="M30" s="17">
         <f>I12</f>
         <v>39446</v>
       </c>
-      <c r="N29">
-        <v>106</v>
-      </c>
-      <c r="O29">
-        <v>106</v>
-      </c>
-      <c r="P29">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="13:16">
-      <c r="M30" s="17"/>
+      <c r="N30">
+        <v>15</v>
+      </c>
+      <c r="O30">
+        <v>15</v>
+      </c>
+      <c r="P30">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="13:16">
       <c r="M31" s="17"/>
@@ -2061,7 +2033,7 @@
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D12 D5:D11" formulaRange="1"/>
-    <ignoredError sqref="M8" formula="1"/>
+    <ignoredError sqref="M9" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Subo el informe con un analisis del 2.7.1 y la curva que faltaba. Si alguno puede revisar buenisimo.
Alguien puede imprimir a color?
</commit_message>
<xml_diff>
--- a/ejercicios/Indicadores/2.1.7.xlsx
+++ b/ejercicios/Indicadores/2.1.7.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Consultas</t>
   </si>
@@ -84,7 +84,13 @@
     <t>FC QC estimado</t>
   </si>
   <si>
-    <t>FC usuario estimado</t>
+    <t>Fecha estimada de liberación al cliente</t>
+  </si>
+  <si>
+    <t>FC liberación usuario estimado</t>
+  </si>
+  <si>
+    <t>FC aceptación usuario estimado</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>FC!$M$4:$M$30</c:f>
+              <c:f>FC!$M$4:$M$35</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>38718</c:v>
                 </c:pt>
@@ -431,10 +437,10 @@
                   <c:v>39293</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>39295</c:v>
+                  <c:v>39301</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39301</c:v>
+                  <c:v>39309</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>39326</c:v>
@@ -447,16 +453,31 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>39446</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38814</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38822</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>38913</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39081</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FC!$N$4:$N$30</c:f>
+              <c:f>FC!$N$4:$N$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -536,6 +557,21 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -561,10 +597,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>FC!$M$4:$M$30</c:f>
+              <c:f>FC!$M$4:$M$35</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>38718</c:v>
                 </c:pt>
@@ -629,10 +665,10 @@
                   <c:v>39293</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>39295</c:v>
+                  <c:v>39301</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39301</c:v>
+                  <c:v>39309</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>39326</c:v>
@@ -645,16 +681,31 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>39446</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38814</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38822</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>38913</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39081</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FC!$O$4:$O$30</c:f>
+              <c:f>FC!$O$4:$O$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -734,6 +785,21 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -749,7 +815,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FC usuario estimado</c:v>
+                  <c:v>FC liberación usuario estimado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -759,10 +825,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>FC!$M$4:$M$30</c:f>
+              <c:f>FC!$M$4:$M$35</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>38718</c:v>
                 </c:pt>
@@ -827,10 +893,10 @@
                   <c:v>39293</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>39295</c:v>
+                  <c:v>39301</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39301</c:v>
+                  <c:v>39309</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>39326</c:v>
@@ -843,16 +909,31 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>39446</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38814</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38822</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>38913</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39081</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FC!$P$4:$P$30</c:f>
+              <c:f>FC!$P$4:$P$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -932,6 +1013,249 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FC!$Q$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FC aceptación usuario estimado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>FC!$M$4:$M$35</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>38718</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38790</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38806</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38808</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38817</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38838</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38852</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38910</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38930</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39071</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39097</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39216</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39223</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39265</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39279</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39284</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39293</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39301</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39309</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39326</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39386</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39428</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39446</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38814</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38822</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>38913</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39081</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39431</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FC!$Q$4:$Q$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -939,24 +1263,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="59599872"/>
-        <c:axId val="59626240"/>
+        <c:axId val="49368064"/>
+        <c:axId val="49390336"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="59599872"/>
+        <c:axId val="49368064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59626240"/>
+        <c:crossAx val="49390336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="59626240"/>
+        <c:axId val="49390336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,7 +1288,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59599872"/>
+        <c:crossAx val="49368064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -977,7 +1301,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1305,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1316,8 +1640,9 @@
     <col min="6" max="6" width="14.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19">
@@ -1349,11 +1674,14 @@
         <v>15</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>17</v>
       </c>
+      <c r="K3" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="M3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1364,7 +1692,10 @@
         <v>21</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="R3"/>
       <c r="S3"/>
@@ -1388,10 +1719,13 @@
         <v>38806</v>
       </c>
       <c r="H4" s="9"/>
-      <c r="I4" s="11">
+      <c r="I4" s="12">
+        <v>38814</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11">
         <v>38838</v>
       </c>
-      <c r="J4" s="10"/>
       <c r="M4" s="17">
         <v>38718</v>
       </c>
@@ -1402,6 +1736,9 @@
         <v>0</v>
       </c>
       <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4" s="17"/>
@@ -1426,9 +1763,12 @@
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="12">
+        <v>38814</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="12">
         <v>38838</v>
       </c>
-      <c r="J5" s="4"/>
       <c r="M5" s="17">
         <f>E4</f>
         <v>38790</v>
@@ -1442,6 +1782,9 @@
       <c r="P5">
         <v>0</v>
       </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
       <c r="R5" s="17"/>
     </row>
     <row r="6" spans="2:19">
@@ -1464,9 +1807,12 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="12">
+        <v>38822</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="12">
         <v>38852</v>
       </c>
-      <c r="J6" s="4"/>
       <c r="M6" s="17">
         <f>E5</f>
         <v>38797</v>
@@ -1480,6 +1826,9 @@
       <c r="P6">
         <v>0</v>
       </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
       <c r="R6" s="17"/>
     </row>
     <row r="7" spans="2:19">
@@ -1502,9 +1851,12 @@
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="12">
+        <v>38913</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="12">
         <v>38930</v>
       </c>
-      <c r="J7" s="4"/>
       <c r="M7" s="17">
         <f>G5</f>
         <v>38804</v>
@@ -1518,6 +1870,9 @@
       <c r="P7">
         <v>0</v>
       </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
       <c r="R7" s="17"/>
     </row>
     <row r="8" spans="2:19">
@@ -1540,9 +1895,12 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="12">
+        <v>39081</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="12">
         <v>39097</v>
       </c>
-      <c r="J8" s="4"/>
       <c r="M8" s="17">
         <f>G4</f>
         <v>38806</v>
@@ -1556,6 +1914,9 @@
       <c r="P8">
         <v>0</v>
       </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
       <c r="R8" s="17"/>
     </row>
     <row r="9" spans="2:19">
@@ -1578,9 +1939,12 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="12">
+        <v>39293</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="12">
         <v>39326</v>
       </c>
-      <c r="J9" s="4"/>
       <c r="M9" s="17">
         <f>E6</f>
         <v>38808</v>
@@ -1594,6 +1958,9 @@
       <c r="P9">
         <v>0</v>
       </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
       <c r="R9" s="17"/>
     </row>
     <row r="10" spans="2:19">
@@ -1616,9 +1983,12 @@
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="12">
-        <v>39295</v>
+        <v>39293</v>
       </c>
       <c r="J10" s="4"/>
+      <c r="K10" s="12">
+        <v>39301</v>
+      </c>
       <c r="M10" s="17">
         <f>G6</f>
         <v>38817</v>
@@ -1632,6 +2002,9 @@
       <c r="P10">
         <v>0</v>
       </c>
+      <c r="Q10">
+        <v>2</v>
+      </c>
       <c r="R10" s="17"/>
     </row>
     <row r="11" spans="2:19">
@@ -1657,8 +2030,11 @@
         <v>39301</v>
       </c>
       <c r="J11" s="4"/>
+      <c r="K11" s="12">
+        <v>39309</v>
+      </c>
       <c r="M11" s="17">
-        <f>I4</f>
+        <f>K4</f>
         <v>38838</v>
       </c>
       <c r="N11">
@@ -1669,6 +2045,9 @@
       </c>
       <c r="P11">
         <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>3</v>
       </c>
       <c r="R11" s="17"/>
     </row>
@@ -1691,12 +2070,15 @@
         <v>39428</v>
       </c>
       <c r="H12" s="6"/>
-      <c r="I12" s="16">
+      <c r="I12" s="12">
+        <v>39431</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="16">
         <v>39446</v>
       </c>
-      <c r="J12" s="7"/>
       <c r="M12" s="17">
-        <f>I6</f>
+        <f>K6</f>
         <v>38852</v>
       </c>
       <c r="N12">
@@ -1706,6 +2088,9 @@
         <v>3</v>
       </c>
       <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
         <v>3</v>
       </c>
       <c r="R12" s="17"/>
@@ -1724,6 +2109,9 @@
       <c r="P13">
         <v>3</v>
       </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="2:19">
       <c r="M14" s="17">
@@ -1739,10 +2127,13 @@
       <c r="P14">
         <v>3</v>
       </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="2:19">
       <c r="M15" s="17">
-        <f>I7</f>
+        <f>K7</f>
         <v>38930</v>
       </c>
       <c r="N15">
@@ -1752,6 +2143,9 @@
         <v>5</v>
       </c>
       <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15">
         <v>5</v>
       </c>
     </row>
@@ -1769,8 +2163,11 @@
       <c r="P16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="13:16">
+      <c r="Q16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="13:17">
       <c r="M17" s="17">
         <f>G8</f>
         <v>39071</v>
@@ -1784,10 +2181,13 @@
       <c r="P17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="13:16">
+      <c r="Q17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="13:17">
       <c r="M18" s="17">
-        <f>I8</f>
+        <f>K8</f>
         <v>39097</v>
       </c>
       <c r="N18">
@@ -1799,8 +2199,11 @@
       <c r="P18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="13:16">
+      <c r="Q18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="13:17">
       <c r="M19" s="17">
         <f>E9</f>
         <v>39216</v>
@@ -1814,8 +2217,11 @@
       <c r="P19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="13:16">
+      <c r="Q19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="13:17">
       <c r="M20" s="17">
         <f>E10</f>
         <v>39223</v>
@@ -1829,8 +2235,11 @@
       <c r="P20">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="13:16">
+      <c r="Q20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="13:17">
       <c r="M21" s="17">
         <f>E11</f>
         <v>39265</v>
@@ -1844,8 +2253,11 @@
       <c r="P21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="13:16">
+      <c r="Q21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="13:17">
       <c r="M22" s="17">
         <f>G9</f>
         <v>39279</v>
@@ -1859,8 +2271,11 @@
       <c r="P22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="13:16">
+      <c r="Q22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="13:17">
       <c r="M23" s="17">
         <f>G10</f>
         <v>39284</v>
@@ -1874,8 +2289,11 @@
       <c r="P23">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="13:16">
+      <c r="Q23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="13:17">
       <c r="M24" s="17">
         <f>G11</f>
         <v>39293</v>
@@ -1889,11 +2307,14 @@
       <c r="P24">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="13:16">
+      <c r="Q24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="13:17">
       <c r="M25" s="17">
-        <f>I10</f>
-        <v>39295</v>
+        <f>K10</f>
+        <v>39301</v>
       </c>
       <c r="N25">
         <v>12</v>
@@ -1904,11 +2325,14 @@
       <c r="P25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="13:16">
+      <c r="Q25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="13:17">
       <c r="M26" s="17">
-        <f>I11</f>
-        <v>39301</v>
+        <f>K11</f>
+        <v>39309</v>
       </c>
       <c r="N26">
         <v>12</v>
@@ -1919,10 +2343,13 @@
       <c r="P26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="13:16">
+      <c r="Q26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="13:17">
       <c r="M27" s="17">
-        <f>I9</f>
+        <f>K9</f>
         <v>39326</v>
       </c>
       <c r="N27">
@@ -1934,8 +2361,11 @@
       <c r="P27">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="13:16">
+      <c r="Q27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="13:17">
       <c r="M28" s="17">
         <f>E12</f>
         <v>39386</v>
@@ -1949,8 +2379,11 @@
       <c r="P28">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="13:16">
+      <c r="Q28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="13:17">
       <c r="M29" s="17">
         <f>G12</f>
         <v>39428</v>
@@ -1964,10 +2397,13 @@
       <c r="P29">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="13:16">
+      <c r="Q29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="13:17">
       <c r="M30" s="17">
-        <f>I12</f>
+        <f>K12</f>
         <v>39446</v>
       </c>
       <c r="N30">
@@ -1979,53 +2415,122 @@
       <c r="P30">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="13:16">
-      <c r="M31" s="17"/>
-    </row>
-    <row r="32" spans="13:16">
-      <c r="M32" s="17"/>
-    </row>
-    <row r="33" spans="13:13">
-      <c r="M33" s="17"/>
-    </row>
-    <row r="34" spans="13:13">
-      <c r="M34" s="17"/>
-    </row>
-    <row r="35" spans="13:13">
-      <c r="M35" s="17"/>
-    </row>
-    <row r="36" spans="13:13">
-      <c r="M36" s="17"/>
-    </row>
-    <row r="37" spans="13:13">
-      <c r="M37" s="17"/>
-    </row>
-    <row r="38" spans="13:13">
-      <c r="M38" s="17"/>
-    </row>
-    <row r="39" spans="13:13">
+      <c r="Q30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="13:17">
+      <c r="M31" s="17">
+        <f>I5</f>
+        <v>38814</v>
+      </c>
+      <c r="N31">
+        <v>3</v>
+      </c>
+      <c r="O31">
+        <v>2</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="13:17">
+      <c r="M32" s="17">
+        <f>I6</f>
+        <v>38822</v>
+      </c>
+      <c r="N32">
+        <v>3</v>
+      </c>
+      <c r="O32">
+        <v>3</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="13:17">
+      <c r="M33" s="17">
+        <f>I7</f>
+        <v>38913</v>
+      </c>
+      <c r="N33">
+        <v>5</v>
+      </c>
+      <c r="O33">
+        <v>5</v>
+      </c>
+      <c r="P33">
+        <v>3</v>
+      </c>
+      <c r="Q33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="13:17">
+      <c r="M34" s="17">
+        <f>I8</f>
+        <v>39081</v>
+      </c>
+      <c r="N34">
+        <v>7</v>
+      </c>
+      <c r="O34">
+        <v>7</v>
+      </c>
+      <c r="P34">
+        <v>5</v>
+      </c>
+      <c r="Q34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="13:17">
+      <c r="M35" s="17">
+        <f>I12</f>
+        <v>39431</v>
+      </c>
+      <c r="N35">
+        <v>15</v>
+      </c>
+      <c r="O35">
+        <v>15</v>
+      </c>
+      <c r="P35">
+        <v>12</v>
+      </c>
+      <c r="Q35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="13:17">
       <c r="M39" s="17"/>
     </row>
-    <row r="40" spans="13:13">
+    <row r="40" spans="13:17">
       <c r="M40" s="17"/>
     </row>
-    <row r="41" spans="13:13">
+    <row r="41" spans="13:17">
       <c r="M41" s="17"/>
     </row>
-    <row r="42" spans="13:13">
+    <row r="42" spans="13:17">
       <c r="M42" s="17"/>
     </row>
-    <row r="43" spans="13:13">
+    <row r="43" spans="13:17">
       <c r="M43" s="17"/>
     </row>
-    <row r="44" spans="13:13">
+    <row r="44" spans="13:17">
       <c r="M44" s="17"/>
     </row>
-    <row r="45" spans="13:13">
+    <row r="45" spans="13:17">
       <c r="M45" s="17"/>
     </row>
-    <row r="46" spans="13:13">
+    <row r="46" spans="13:17">
       <c r="M46" s="17"/>
     </row>
   </sheetData>
@@ -2033,7 +2538,6 @@
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D12 D5:D11" formulaRange="1"/>
-    <ignoredError sqref="M9" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>